<commit_message>
added base screenshots Folder
</commit_message>
<xml_diff>
--- a/Data Files/data.xlsx
+++ b/Data Files/data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sudhak\Katalon Studio\Panopticon\Data Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{624731FC-B042-4F57-AF85-D5B2C284FC0C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8BE6079-2DE9-43BA-9808-24EA4FF48A54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="42">
   <si>
     <t>TestCaseName</t>
   </si>
@@ -63,61 +63,115 @@
 table.</t>
   </si>
   <si>
-    <t>workbook/visualization 
+    <t>workbook1</t>
+  </si>
+  <si>
+    <t>workbook2</t>
+  </si>
+  <si>
+    <t>workbook3</t>
+  </si>
+  <si>
+    <t>workbook4</t>
+  </si>
+  <si>
+    <t>D:\\StocksTimeSeries_2020.xls</t>
+  </si>
+  <si>
+    <t>D:\\StocksStatic_2020-02-12-16-36-31.xls</t>
+  </si>
+  <si>
+    <t>scrollElement-visualization.LineGraph1</t>
+  </si>
+  <si>
+    <t>scrollElement-visualization.VerticalBarGraph1</t>
+  </si>
+  <si>
+    <t>graphlocation</t>
+  </si>
+  <si>
+    <t>columnname</t>
+  </si>
+  <si>
+    <t>Calculated</t>
+  </si>
+  <si>
+    <t>Ranking</t>
+  </si>
+  <si>
+    <t>Time Bucket</t>
+  </si>
+  <si>
+    <t>Verify the workbook/visualization 
 features for a non time 
 series data table having 
 Time bucket.</t>
   </si>
   <si>
-    <t>workbook1</t>
-  </si>
-  <si>
-    <t>workbook2</t>
-  </si>
-  <si>
-    <t>workbook3</t>
-  </si>
-  <si>
-    <t>workbook4</t>
-  </si>
-  <si>
-    <t>D:\\StocksTimeSeries_2020.xls</t>
-  </si>
-  <si>
-    <t>D:\\StocksStatic_2020-02-12-16-36-31.xls</t>
-  </si>
-  <si>
-    <t>scrollElement-visualization.LineGraph1</t>
-  </si>
-  <si>
-    <t>scrollElement-visualization.VerticalBarGraph1</t>
-  </si>
-  <si>
-    <t>graphlocation</t>
-  </si>
-  <si>
-    <t>D:\\copydata\\screenshots\\graph1.png</t>
-  </si>
-  <si>
-    <t>D:\\copydata\\screenshots\\graph2.png</t>
-  </si>
-  <si>
-    <t>D:\\copydata\\screenshots\\graph3.png</t>
-  </si>
-  <si>
-    <t>D:\\copydata\\screenshots\\graph4.png</t>
-  </si>
-  <si>
-    <t>columnname</t>
-  </si>
-  <si>
-    <t>Calculated</t>
-  </si>
-  <si>
-    <t>Ranking</t>
-  </si>
-  <si>
-    <t>Time Bucket</t>
+    <t>workbook5</t>
+  </si>
+  <si>
+    <t>UserChoice</t>
+  </si>
+  <si>
+    <t>workbook6</t>
+  </si>
+  <si>
+    <t>MQTT</t>
+  </si>
+  <si>
+    <t>graph1</t>
+  </si>
+  <si>
+    <t>graph2</t>
+  </si>
+  <si>
+    <t>graph3</t>
+  </si>
+  <si>
+    <t>graph4</t>
+  </si>
+  <si>
+    <t>SUM_TIMEWIN("Adj Close", [TimeWindowStart],[TimeWindowEnd])</t>
+  </si>
+  <si>
+    <t>Expression</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[Adj_Close]+[Holding] </t>
+  </si>
+  <si>
+    <t>KDB</t>
+  </si>
+  <si>
+    <t>workbook7</t>
+  </si>
+  <si>
+    <t>Verify the workbook/visualization for a timeseries visualization having Calculated column added to it for MQTT connector</t>
+  </si>
+  <si>
+    <t>Verify the workbook/visualization 
+features for a non time 
+series data table having 
+having Calculated Column for KDB connector</t>
+  </si>
+  <si>
+    <t>Verify the workbook/visualization features for a non time series data table having Time bucket for KDB connector</t>
+  </si>
+  <si>
+    <t>workbook8</t>
+  </si>
+  <si>
+    <t>graph5</t>
+  </si>
+  <si>
+    <t>graph6</t>
+  </si>
+  <si>
+    <t>graph7</t>
+  </si>
+  <si>
+    <t>Verify the workbook/visualization for a timeseries visualization having Ranking column added to it for KDB connector</t>
   </si>
 </sst>
 </file>
@@ -444,10 +498,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView tabSelected="1" topLeftCell="B5" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -458,9 +512,11 @@
     <col min="4" max="4" width="42.33203125" customWidth="1"/>
     <col min="5" max="5" width="33.88671875" customWidth="1"/>
     <col min="6" max="6" width="16.5546875" customWidth="1"/>
+    <col min="7" max="7" width="13.109375" customWidth="1"/>
+    <col min="8" max="8" width="20.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -474,88 +530,178 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" t="s">
         <v>16</v>
       </c>
-      <c r="F1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="G1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2" t="s">
         <v>17</v>
       </c>
-      <c r="F2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="H2" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3" t="s">
         <v>18</v>
       </c>
-      <c r="F3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" t="s">
         <v>10</v>
       </c>
-      <c r="C4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="D5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F5" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5" t="s">
-        <v>20</v>
-      </c>
-      <c r="F5" t="s">
+    <row r="6" spans="1:8" ht="72" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" t="s">
+        <v>38</v>
+      </c>
+      <c r="F6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" t="s">
+        <v>17</v>
+      </c>
+      <c r="G7" t="s">
         <v>24</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" t="s">
+        <v>39</v>
+      </c>
+      <c r="F8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D9" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" t="s">
+        <v>40</v>
+      </c>
+      <c r="F9" t="s">
+        <v>19</v>
+      </c>
+      <c r="G9" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>